<commit_message>
Added some minor modifications
</commit_message>
<xml_diff>
--- a/RPAFramework/RoboticEnterpriseFramework/Data/Input/Songs.xlsx
+++ b/RPAFramework/RoboticEnterpriseFramework/Data/Input/Songs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura-elena.olaru/Downloads/RPA/GIT/YoutubePlaylistCreator/RPAFramework/RoboticEnterpriseFramework/Data/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Desktop\RPA\ProiectRPA\YoutubePlaylistCreator\RPAFramework\RoboticEnterpriseFramework\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EEA0F5-4A4B-0844-9D7C-9F3E8FC1A373}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FA1DEB-6670-4FFB-B52A-46B103DF8DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,10 +63,10 @@
     <t>Alcest</t>
   </si>
   <si>
-    <t>GloriaJeans</t>
-  </si>
-  <si>
-    <t>Starbucks</t>
+    <t>Starbucks1</t>
+  </si>
+  <si>
+    <t>GloriaJeans1</t>
   </si>
   <si>
     <t>Unlisted</t>
@@ -390,16 +390,16 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -410,7 +410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -421,7 +421,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -432,7 +432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -443,23 +443,23 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>

</xml_diff>